<commit_message>
worked on formatting worksheetas like royaltyworksheet.py
</commit_message>
<xml_diff>
--- a/excel-app/files/database.xlsx
+++ b/excel-app/files/database.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\python-playground\excel-app\database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="7305" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="4320" yWindow="4820" windowWidth="24660" windowHeight="13240" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Roy Module Construct" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,12 @@
     <sheet name="ProductClauses" sheetId="7" r:id="rId13"/>
     <sheet name="ECONData" sheetId="10" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -678,7 +678,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -748,7 +748,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -759,27 +759,27 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -787,23 +787,23 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -811,14 +811,14 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -827,7 +827,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -908,10 +908,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="8" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -923,10 +923,10 @@
     <xf numFmtId="14" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="8" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="8" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1052,7 +1052,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1107,7 +1107,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1162,7 +1162,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1217,7 +1217,7 @@
         </a:prstGeom>
         <a:noFill/>
         <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
@@ -1275,7 +1275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1310,7 +1310,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1519,40 +1519,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="17">
         <f>221.123456 - 2.123456</f>
         <v>219</v>
@@ -1570,12 +1570,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="F6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="14.5" customHeight="1">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="14" t="s">
         <v>3</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="14" t="s">
         <v>2</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="14" t="s">
         <v>7</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="14"/>
       <c r="B11" s="4"/>
       <c r="C11" s="6"/>
@@ -1691,7 +1691,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="14"/>
       <c r="B12" s="4"/>
       <c r="C12" s="6"/>
@@ -1703,7 +1703,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="14"/>
       <c r="B13" s="4"/>
       <c r="C13" s="6"/>
@@ -1715,7 +1715,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="14"/>
       <c r="B14" s="4"/>
       <c r="C14" s="6"/>
@@ -1727,7 +1727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15" thickBot="1">
       <c r="A15" s="15"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
@@ -1737,22 +1737,22 @@
       <c r="G15" s="9"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="C22" t="s">
         <v>43</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="C23" t="s">
         <v>44</v>
       </c>
@@ -1768,17 +1768,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="D24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="D25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="C28" s="21">
         <v>42307</v>
       </c>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="B29" s="22"/>
       <c r="C29" s="21">
         <v>42307</v>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="H29" s="25"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="B30" s="22"/>
       <c r="C30" s="21">
         <v>42282</v>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="H30" s="25"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15" thickBot="1">
       <c r="B31" s="26"/>
       <c r="C31" s="27">
         <v>42282</v>
@@ -1853,8 +1853,8 @@
       </c>
       <c r="H31" s="30"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15" thickTop="1"/>
+    <row r="33" spans="5:5">
       <c r="E33">
         <f>SUM(E27:E32)</f>
         <v>19815.62</v>
@@ -1868,8 +1868,13 @@
     <hyperlink ref="F31" r:id="rId4" display="https://qbo-ca.onlinepayroll.intuit.com/reports/checkRegister.jsf?directAccess=true"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <drawing r:id="rId5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1881,9 +1886,9 @@
       <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1965,6 +1970,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1976,12 +1986,12 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -1992,7 +2002,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2005,6 +2015,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2016,12 +2031,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -2031,6 +2046,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2042,19 +2062,19 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -2082,6 +2102,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2090,23 +2115,22 @@
   <dimension ref="A1:AE48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -2201,7 +2225,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -2296,7 +2320,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -2391,7 +2415,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -2486,7 +2510,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -2581,7 +2605,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -2676,7 +2700,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -2771,7 +2795,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -2866,7 +2890,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -2961,7 +2985,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -3056,7 +3080,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -3151,7 +3175,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -3246,7 +3270,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -3341,7 +3365,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -3436,7 +3460,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -3531,7 +3555,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -3626,7 +3650,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
         <v>89</v>
       </c>
@@ -3721,7 +3745,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -3816,7 +3840,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31">
       <c r="A19" t="s">
         <v>98</v>
       </c>
@@ -3911,7 +3935,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
         <v>92</v>
       </c>
@@ -4006,7 +4030,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -4101,7 +4125,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -4196,7 +4220,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
         <v>95</v>
       </c>
@@ -4291,7 +4315,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
         <v>96</v>
       </c>
@@ -4386,7 +4410,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -4481,7 +4505,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -4576,7 +4600,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -4671,7 +4695,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -4766,7 +4790,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31">
       <c r="A29" t="s">
         <v>89</v>
       </c>
@@ -4861,7 +4885,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31">
       <c r="A30" t="s">
         <v>90</v>
       </c>
@@ -4956,7 +4980,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31">
       <c r="A31" t="s">
         <v>91</v>
       </c>
@@ -5051,7 +5075,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -5146,7 +5170,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -5241,7 +5265,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -5336,7 +5360,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -5431,7 +5455,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -5526,7 +5550,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -5621,7 +5645,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -5716,7 +5740,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
         <v>81</v>
       </c>
@@ -5811,7 +5835,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -5906,7 +5930,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31">
       <c r="A41" t="s">
         <v>89</v>
       </c>
@@ -6001,7 +6025,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -6096,7 +6120,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:31">
       <c r="A43" t="s">
         <v>91</v>
       </c>
@@ -6191,7 +6215,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31">
       <c r="A44" t="s">
         <v>92</v>
       </c>
@@ -6286,7 +6310,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31">
       <c r="A45" t="s">
         <v>93</v>
       </c>
@@ -6381,7 +6405,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -6476,7 +6500,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:31">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -6571,7 +6595,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:31">
       <c r="A48" t="s">
         <v>96</v>
       </c>
@@ -6668,6 +6692,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6679,15 +6708,15 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>152</v>
       </c>
@@ -6698,7 +6727,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>153</v>
       </c>
@@ -6709,7 +6738,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -6722,6 +6751,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6730,16 +6764,16 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>168</v>
       </c>
@@ -6750,7 +6784,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="28">
       <c r="A2" t="s">
         <v>177</v>
       </c>
@@ -6763,6 +6797,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6774,19 +6813,19 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" customWidth="1"/>
+    <col min="10" max="10" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="19" t="s">
         <v>52</v>
       </c>
@@ -6821,7 +6860,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6853,7 +6892,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6882,7 +6921,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -6908,7 +6947,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -6934,7 +6973,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -6954,7 +6993,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -6977,7 +7016,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -7000,7 +7039,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -7023,7 +7062,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -7043,7 +7082,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -7068,6 +7107,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7079,15 +7123,15 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="19" t="s">
         <v>52</v>
       </c>
@@ -7107,7 +7151,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -7124,7 +7168,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7141,7 +7185,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -7158,7 +7202,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -7175,7 +7219,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -7192,7 +7236,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -7209,7 +7253,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -7226,7 +7270,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -7243,7 +7287,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -7260,7 +7304,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -7282,6 +7326,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7289,24 +7338,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -7344,7 +7393,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7382,7 +7431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7420,7 +7469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7452,7 +7501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7484,7 +7533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7513,7 +7562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7548,7 +7597,7 @@
         <v>41974</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7583,7 +7632,7 @@
         <v>41974</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7618,7 +7667,7 @@
         <v>41974</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7650,7 +7699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>10</v>
       </c>
@@ -7682,7 +7731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>11</v>
       </c>
@@ -7714,7 +7763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>12</v>
       </c>
@@ -7746,7 +7795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>13</v>
       </c>
@@ -7778,7 +7827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>14</v>
       </c>
@@ -7810,7 +7859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>15</v>
       </c>
@@ -7842,7 +7891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>16</v>
       </c>
@@ -7874,7 +7923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>17</v>
       </c>
@@ -7906,7 +7955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>18</v>
       </c>
@@ -7938,7 +7987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>19</v>
       </c>
@@ -7970,7 +8019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>20</v>
       </c>
@@ -8002,7 +8051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8034,7 +8083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>22</v>
       </c>
@@ -8066,7 +8115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>23</v>
       </c>
@@ -8098,7 +8147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>24</v>
       </c>
@@ -8130,7 +8179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>25</v>
       </c>
@@ -8162,7 +8211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>30</v>
       </c>
@@ -8194,7 +8243,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>31</v>
       </c>
@@ -8220,7 +8269,7 @@
         <v>40513</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>32</v>
       </c>
@@ -8246,7 +8295,7 @@
         <v>40513</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>33</v>
       </c>
@@ -8272,7 +8321,7 @@
         <v>41974</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>1000</v>
       </c>
@@ -8298,7 +8347,7 @@
         <v>41609</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>2000</v>
       </c>
@@ -8330,7 +8379,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>2001</v>
       </c>
@@ -8362,7 +8411,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>3000</v>
       </c>
@@ -8390,7 +8439,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8398,25 +8452,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>130</v>
       </c>
@@ -8454,7 +8508,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8477,7 +8531,7 @@
         <v>740</v>
       </c>
       <c r="H2">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="I2">
         <v>2.2000000000000002</v>
@@ -8492,7 +8546,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8530,7 +8584,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8568,7 +8622,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8606,7 +8660,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>34</v>
       </c>
@@ -8644,7 +8698,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>35</v>
       </c>
@@ -8682,7 +8736,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>1</v>
       </c>
@@ -8720,7 +8774,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>2</v>
       </c>
@@ -8758,7 +8812,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>3</v>
       </c>
@@ -8796,7 +8850,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>4</v>
       </c>
@@ -8834,7 +8888,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>5</v>
       </c>
@@ -8872,7 +8926,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>7</v>
       </c>
@@ -8910,7 +8964,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>8</v>
       </c>
@@ -8948,7 +9002,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>9</v>
       </c>
@@ -8986,7 +9040,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>10</v>
       </c>
@@ -9024,7 +9078,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>11</v>
       </c>
@@ -9062,7 +9116,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>12</v>
       </c>
@@ -9100,7 +9154,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>13</v>
       </c>
@@ -9138,7 +9192,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>14</v>
       </c>
@@ -9176,7 +9230,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>15</v>
       </c>
@@ -9214,7 +9268,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>16</v>
       </c>
@@ -9252,7 +9306,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>17</v>
       </c>
@@ -9290,7 +9344,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>18</v>
       </c>
@@ -9328,7 +9382,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>19</v>
       </c>
@@ -9366,7 +9420,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>20</v>
       </c>
@@ -9404,7 +9458,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>21</v>
       </c>
@@ -9442,7 +9496,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>22</v>
       </c>
@@ -9480,7 +9534,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>23</v>
       </c>
@@ -9518,7 +9572,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>24</v>
       </c>
@@ -9556,7 +9610,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>25</v>
       </c>
@@ -9594,7 +9648,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>26</v>
       </c>
@@ -9632,7 +9686,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>27</v>
       </c>
@@ -9670,7 +9724,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>28</v>
       </c>
@@ -9708,7 +9762,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>29</v>
       </c>
@@ -9746,7 +9800,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>30</v>
       </c>
@@ -9784,7 +9838,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>31</v>
       </c>
@@ -9822,7 +9876,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>32</v>
       </c>
@@ -9860,7 +9914,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>33</v>
       </c>
@@ -9898,7 +9952,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>36</v>
       </c>
@@ -9936,7 +9990,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>37</v>
       </c>
@@ -9974,7 +10028,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12">
       <c r="A42">
         <v>38</v>
       </c>
@@ -10012,7 +10066,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12">
       <c r="A43">
         <v>39</v>
       </c>
@@ -10050,7 +10104,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>40</v>
       </c>
@@ -10088,7 +10142,7 @@
         <v>0.123455</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>41</v>
       </c>
@@ -10128,6 +10182,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10137,12 +10196,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>130</v>
       </c>
@@ -10180,7 +10239,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10220,6 +10279,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -10229,9 +10293,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -10311,7 +10375,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="A2">
         <v>201501</v>
       </c>
@@ -10388,7 +10452,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="A3">
         <v>201501</v>
       </c>
@@ -10465,7 +10529,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="A4">
         <v>201501</v>
       </c>
@@ -10542,7 +10606,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="A5">
         <v>201501</v>
       </c>
@@ -10616,7 +10680,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26">
       <c r="A6">
         <v>201501</v>
       </c>
@@ -10690,7 +10754,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="A7">
         <v>201501</v>
       </c>
@@ -10761,7 +10825,7 @@
         <v>386.97</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26">
       <c r="A8">
         <v>201501</v>
       </c>
@@ -10832,7 +10896,7 @@
         <v>1597.62</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="A9">
         <v>201501</v>
       </c>
@@ -10903,7 +10967,7 @@
         <v>1152.6099999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26">
       <c r="A10">
         <v>201501</v>
       </c>
@@ -10974,7 +11038,7 @@
         <v>386.97</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="A11">
         <v>201502</v>
       </c>
@@ -11048,7 +11112,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26">
       <c r="A12">
         <v>201503</v>
       </c>
@@ -11122,7 +11186,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26">
       <c r="A13">
         <v>201504</v>
       </c>
@@ -11193,7 +11257,7 @@
         <v>11415.50327125</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26">
       <c r="A14">
         <v>201504</v>
       </c>
@@ -11264,7 +11328,7 @@
         <v>11415.50327125</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="A15">
         <v>201504</v>
       </c>
@@ -11338,7 +11402,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="A16">
         <v>201503</v>
       </c>
@@ -11412,7 +11476,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26">
       <c r="A17">
         <v>201503</v>
       </c>
@@ -11489,7 +11553,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26">
       <c r="A18">
         <v>201503</v>
       </c>
@@ -11566,7 +11630,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26">
       <c r="A19">
         <v>201503</v>
       </c>
@@ -11643,7 +11707,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26">
       <c r="A20">
         <v>201503</v>
       </c>
@@ -11720,7 +11784,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26">
       <c r="A21">
         <v>201504</v>
       </c>
@@ -11797,7 +11861,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26">
       <c r="A22">
         <v>201504</v>
       </c>
@@ -11874,7 +11938,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26">
       <c r="A23">
         <v>201504</v>
       </c>
@@ -11951,7 +12015,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26">
       <c r="A24">
         <v>201504</v>
       </c>
@@ -12022,7 +12086,7 @@
         <v>3607.43</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26">
       <c r="A25">
         <v>201504</v>
       </c>
@@ -12093,7 +12157,7 @@
         <v>3607.43</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26">
       <c r="A26">
         <v>201504</v>
       </c>
@@ -12167,7 +12231,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26">
       <c r="A27">
         <v>201504</v>
       </c>
@@ -12241,7 +12305,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26">
       <c r="A28">
         <v>201504</v>
       </c>
@@ -12312,7 +12376,7 @@
         <v>6080.8999749999994</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26">
       <c r="A29">
         <v>201504</v>
       </c>
@@ -12383,7 +12447,7 @@
         <v>5925.68</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26">
       <c r="A30">
         <v>201504</v>
       </c>
@@ -12457,7 +12521,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26">
       <c r="A31">
         <v>201504</v>
       </c>
@@ -12530,5 +12594,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>